<commit_message>
Initial commit: add survey files
</commit_message>
<xml_diff>
--- a/docs/MRT_stu_codes_0515.xlsx
+++ b/docs/MRT_stu_codes_0515.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoonj\AppData\Local\Programs\Python\Python311\Code\Random ID_STU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoonj\OneDrive\바탕 화면\To do\Survey_0516_mod\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D725FD01-6FB2-4092-B8D8-752B2FF57FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62CA9B3-32E0-405F-9ED5-B10DA2767C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
   <si>
     <t>code</t>
   </si>
@@ -174,13 +174,37 @@
   </si>
   <si>
     <t>MRTKfcu</t>
+  </si>
+  <si>
+    <t>MRTI019</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRT3NS2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRTV702</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRTD3AN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRTjvoY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRTKfcu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +221,21 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -238,11 +277,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -816,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -1043,38 +1084,38 @@
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A45" t="s">
-        <v>44</v>
+      <c r="A45" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A46" t="s">
-        <v>45</v>
+      <c r="A46" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A47" t="s">
-        <v>46</v>
+      <c r="A47" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A48" t="s">
-        <v>47</v>
+      <c r="A48" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A49" t="s">
+      <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A50" t="s">
-        <v>49</v>
+      <c r="A50" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A51" t="s">
-        <v>50</v>
+      <c r="A51" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>